<commit_message>
Time Tracking update 5/15
updated last weeks and what I worked on Sunday/Today
</commit_message>
<xml_diff>
--- a/TimeTrackingDocument/CS297-TimeTracking.xlsx
+++ b/TimeTrackingDocument/CS297-TimeTracking.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -621,11 +621,11 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>3.5</v>
+        <v>10.5</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -644,9 +644,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,7 +670,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -688,7 +691,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -709,7 +712,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the island 3 and time sheet
Did the things
</commit_message>
<xml_diff>
--- a/TimeTrackingDocument/CS297-TimeTracking.xlsx
+++ b/TimeTrackingDocument/CS297-TimeTracking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CapstoneStuff\IslandAdventureCapstone\TimeTrackingDocument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\IslandAdventureCapstone\TimeTrackingDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -528,11 +528,11 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C13" si="1">B6+C5</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -560,13 +560,19 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -584,13 +590,19 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -610,11 +622,14 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -634,11 +649,11 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -658,11 +673,11 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -679,11 +694,11 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -700,11 +715,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
so cat now tracks with player. need to polish
cat tracks with player. time card ujpdated as welll
</commit_message>
<xml_diff>
--- a/TimeTrackingDocument/CS297-TimeTracking.xlsx
+++ b/TimeTrackingDocument/CS297-TimeTracking.xlsx
@@ -685,11 +685,11 @@
         <v>61</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -713,7 +713,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -734,7 +734,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>

</xml_diff>